<commit_message>
& - №71036492 от 22.09.2024 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/San_Marino/#EURO#San_Marino#Commemorative#[2004-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/San_Marino/#EURO#San_Marino#Commemorative#[2004-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\San_Marino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161D1954-370B-44EB-B108-C084589F1796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A760B50A-8B67-43EB-91F6-1DACB2E82129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5660" yWindow="1450" windowWidth="28720" windowHeight="19550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -1049,7 +1049,7 @@
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1375,7 +1375,7 @@
         <v>26</v>
       </c>
       <c r="G13" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="10" t="str">
         <f t="shared" si="2"/>
@@ -1825,7 +1825,7 @@
         <v>64</v>
       </c>
       <c r="G31" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="10" t="str">
         <f t="shared" si="7"/>
@@ -1850,7 +1850,7 @@
         <v>64</v>
       </c>
       <c r="G32" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="10" t="str">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
& - 79850809 от 07.07.2025 https://meshok.net/ - 79031149 от 05.06.2025 https://meshok.net/ (2)
</commit_message>
<xml_diff>
--- a/Collections/EURO/San_Marino/#EURO#San_Marino#Commemorative#[2004-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/San_Marino/#EURO#San_Marino#Commemorative#[2004-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\San_Marino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0491B0D2-88FA-4D80-AA30-5C3715DC0E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3630037B-C127-4441-8505-E5AD7E4DF9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5250" yWindow="2150" windowWidth="33150" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -903,18 +903,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -943,6 +931,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -952,6 +952,15 @@
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -976,15 +985,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1006,9 +1006,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="4" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1283,7 +1283,7 @@
       <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M24" sqref="M24"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1299,15 +1299,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="52"/>
+      <c r="D1" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="62"/>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1319,7 +1319,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="50"/>
+      <c r="A2" s="60"/>
       <c r="B2" s="31" t="s">
         <v>67</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="39" t="s">
         <v>77</v>
@@ -1371,24 +1371,24 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="53">
+      <c r="A4" s="49">
         <v>2005</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="56" t="s">
+      <c r="C4" s="51"/>
+      <c r="D4" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="57" t="s">
+      <c r="F4" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="58">
-        <v>0</v>
+      <c r="G4" s="54">
+        <v>1</v>
       </c>
       <c r="H4" s="39"/>
       <c r="I4" s="8" t="str">
@@ -1416,7 +1416,7 @@
       <c r="G5" s="30">
         <v>1</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="58" t="s">
         <v>78</v>
       </c>
       <c r="I5" s="8" t="str">
@@ -1441,7 +1441,7 @@
       <c r="F6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="61">
+      <c r="G6" s="57">
         <v>1</v>
       </c>
       <c r="H6" s="40"/>
@@ -1467,33 +1467,33 @@
       <c r="F7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="59">
-        <v>1</v>
-      </c>
-      <c r="H7" s="60"/>
+      <c r="G7" s="55">
+        <v>1</v>
+      </c>
+      <c r="H7" s="56"/>
       <c r="I7" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="53">
+      <c r="A8" s="49">
         <v>2009</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="57" t="s">
+      <c r="C8" s="51"/>
+      <c r="D8" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="58">
+      <c r="G8" s="54">
         <v>1</v>
       </c>
       <c r="H8" s="40"/>
@@ -1547,7 +1547,7 @@
       <c r="F10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="61">
+      <c r="G10" s="57">
         <v>1</v>
       </c>
       <c r="H10" s="42"/>
@@ -1573,7 +1573,7 @@
       <c r="F11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="59">
+      <c r="G11" s="55">
         <v>1</v>
       </c>
       <c r="H11" s="42"/>
@@ -1583,23 +1583,23 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="53">
+      <c r="A12" s="49">
         <v>2013</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="57" t="s">
+      <c r="C12" s="51"/>
+      <c r="D12" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="58">
+      <c r="G12" s="54">
         <v>1</v>
       </c>
       <c r="H12" s="42"/>
@@ -1653,7 +1653,7 @@
       <c r="F14" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="61">
+      <c r="G14" s="57">
         <v>1</v>
       </c>
       <c r="H14" s="35"/>
@@ -1679,7 +1679,7 @@
       <c r="F15" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="59">
+      <c r="G15" s="55">
         <v>1</v>
       </c>
       <c r="H15" s="35"/>
@@ -1689,23 +1689,23 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="53">
+      <c r="A16" s="49">
         <v>2015</v>
       </c>
-      <c r="B16" s="54" t="s">
+      <c r="B16" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="57" t="s">
+      <c r="C16" s="51"/>
+      <c r="D16" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="58">
+      <c r="G16" s="54">
         <v>1</v>
       </c>
       <c r="H16" s="35"/>
@@ -1759,7 +1759,7 @@
       <c r="F18" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="61">
+      <c r="G18" s="57">
         <v>1</v>
       </c>
       <c r="H18" s="37"/>
@@ -1785,7 +1785,7 @@
       <c r="F19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="59">
+      <c r="G19" s="55">
         <v>1</v>
       </c>
       <c r="H19" s="37"/>
@@ -1795,23 +1795,23 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="53">
+      <c r="A20" s="49">
         <v>2017</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="57" t="s">
+      <c r="C20" s="51"/>
+      <c r="D20" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="58">
+      <c r="G20" s="54">
         <v>1</v>
       </c>
       <c r="H20" s="37"/>
@@ -1865,7 +1865,7 @@
       <c r="F22" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="61">
+      <c r="G22" s="57">
         <v>1</v>
       </c>
       <c r="H22" s="32"/>
@@ -1891,7 +1891,7 @@
       <c r="F23" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="59">
+      <c r="G23" s="55">
         <v>0</v>
       </c>
       <c r="H23" s="32"/>
@@ -1901,23 +1901,23 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="53">
+      <c r="A24" s="49">
         <v>2019</v>
       </c>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="57" t="s">
+      <c r="C24" s="51"/>
+      <c r="D24" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="58">
+      <c r="G24" s="54">
         <v>1</v>
       </c>
       <c r="H24" s="32"/>
@@ -1971,7 +1971,7 @@
       <c r="F26" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="61">
+      <c r="G26" s="57">
         <v>1</v>
       </c>
       <c r="H26" s="33"/>
@@ -1997,7 +1997,7 @@
       <c r="F27" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="59">
+      <c r="G27" s="55">
         <v>1</v>
       </c>
       <c r="H27" s="33"/>
@@ -2007,23 +2007,23 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="53">
+      <c r="A28" s="49">
         <v>2021</v>
       </c>
-      <c r="B28" s="54" t="s">
+      <c r="B28" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="57" t="s">
+      <c r="C28" s="51"/>
+      <c r="D28" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="58">
+      <c r="G28" s="54">
         <v>1</v>
       </c>
       <c r="H28" s="33"/>
@@ -2077,7 +2077,7 @@
       <c r="F30" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="61">
+      <c r="G30" s="57">
         <v>0</v>
       </c>
       <c r="H30" s="45"/>
@@ -2103,7 +2103,7 @@
       <c r="F31" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G31" s="59">
+      <c r="G31" s="55">
         <v>1</v>
       </c>
       <c r="H31" s="45"/>
@@ -2113,23 +2113,23 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="53">
+      <c r="A32" s="49">
         <v>2023</v>
       </c>
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" s="57" t="s">
+      <c r="C32" s="51"/>
+      <c r="D32" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="G32" s="58">
+      <c r="G32" s="54">
         <v>1</v>
       </c>
       <c r="H32" s="45"/>
@@ -2183,7 +2183,7 @@
       <c r="F34" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="61">
+      <c r="G34" s="57">
         <v>1</v>
       </c>
       <c r="H34" s="47"/>
@@ -2209,7 +2209,7 @@
       <c r="F35" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="G35" s="59">
+      <c r="G35" s="55">
         <v>1</v>
       </c>
       <c r="H35" s="47"/>
@@ -2250,7 +2250,7 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="G3:G34">
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G3))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2267,7 +2267,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G35))))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2284,7 +2284,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(G36))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>